<commit_message>
Reestructure project to support Entity Framework 3.1
</commit_message>
<xml_diff>
--- a/docs/Entities.xlsx
+++ b/docs/Entities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JulianSegura\source\repos\Cotix\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BDE6F5-BB6D-4CD0-9FD1-296CAD481BF7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD1D98E-998A-4CBC-B045-A21178523107}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
   <si>
     <t>User</t>
   </si>
@@ -197,10 +197,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,14 +505,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="D2" s="3" t="s">
+      <c r="B2" s="4"/>
+      <c r="D2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -528,7 +528,9 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
@@ -540,7 +542,9 @@
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>17</v>
       </c>
@@ -581,18 +585,18 @@
       <c r="E8" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="D11" s="3" t="s">
+      <c r="B11" s="4"/>
+      <c r="D11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="G11" s="3" t="s">
+      <c r="E11" s="4"/>
+      <c r="G11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="3"/>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -657,10 +661,10 @@
         <v>13</v>
       </c>
       <c r="B16" s="1"/>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
         <v>34</v>
       </c>
       <c r="G16" s="2" t="s">

</xml_diff>